<commit_message>
correct coastal locations that were assigned land for 1deg resolution.  Remove addidental extra field "abev"
</commit_message>
<xml_diff>
--- a/JETZON_MSC_POC-fluxes_Elisa_010925.xlsx
+++ b/JETZON_MSC_POC-fluxes_Elisa_010925.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="93008" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="99290" uniqueCount="681">
   <si>
     <t>Project</t>
   </si>
@@ -6938,10 +6938,14 @@
         <v>576</v>
       </c>
       <c r="R80" s="0">
-        <v>0</v>
-      </c>
-      <c r="S80" s="0"/>
-      <c r="T80" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S80" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T80" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U80" s="0"/>
     </row>
     <row r="81">
@@ -6993,10 +6997,14 @@
         <v>576</v>
       </c>
       <c r="R81" s="0">
-        <v>0</v>
-      </c>
-      <c r="S81" s="0"/>
-      <c r="T81" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S81" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T81" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U81" s="0"/>
     </row>
     <row r="82">
@@ -7048,10 +7056,14 @@
         <v>576</v>
       </c>
       <c r="R82" s="0">
-        <v>0</v>
-      </c>
-      <c r="S82" s="0"/>
-      <c r="T82" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S82" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T82" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U82" s="0"/>
     </row>
     <row r="83">
@@ -7103,10 +7115,14 @@
         <v>576</v>
       </c>
       <c r="R83" s="0">
-        <v>0</v>
-      </c>
-      <c r="S83" s="0"/>
-      <c r="T83" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S83" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T83" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U83" s="0"/>
     </row>
     <row r="84">
@@ -7158,10 +7174,14 @@
         <v>576</v>
       </c>
       <c r="R84" s="0">
-        <v>0</v>
-      </c>
-      <c r="S84" s="0"/>
-      <c r="T84" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S84" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T84" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U84" s="0"/>
     </row>
     <row r="85">
@@ -7213,10 +7233,14 @@
         <v>576</v>
       </c>
       <c r="R85" s="0">
-        <v>0</v>
-      </c>
-      <c r="S85" s="0"/>
-      <c r="T85" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S85" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T85" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U85" s="0"/>
     </row>
     <row r="86">
@@ -7622,10 +7646,14 @@
         <v>576</v>
       </c>
       <c r="R92" s="0">
-        <v>0</v>
-      </c>
-      <c r="S92" s="0"/>
-      <c r="T92" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S92" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T92" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U92" s="0"/>
     </row>
     <row r="93">
@@ -7677,10 +7705,14 @@
         <v>576</v>
       </c>
       <c r="R93" s="0">
-        <v>0</v>
-      </c>
-      <c r="S93" s="0"/>
-      <c r="T93" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S93" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T93" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U93" s="0"/>
     </row>
     <row r="94">
@@ -7732,10 +7764,14 @@
         <v>576</v>
       </c>
       <c r="R94" s="0">
-        <v>0</v>
-      </c>
-      <c r="S94" s="0"/>
-      <c r="T94" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S94" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T94" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U94" s="0"/>
     </row>
     <row r="95">
@@ -7787,10 +7823,14 @@
         <v>576</v>
       </c>
       <c r="R95" s="0">
-        <v>0</v>
-      </c>
-      <c r="S95" s="0"/>
-      <c r="T95" s="0"/>
+        <v>3</v>
+      </c>
+      <c r="S95" s="0" t="s">
+        <v>664</v>
+      </c>
+      <c r="T95" s="0" t="s">
+        <v>672</v>
+      </c>
       <c r="U95" s="0"/>
     </row>
     <row r="96">
@@ -10111,10 +10151,14 @@
         <v>578</v>
       </c>
       <c r="R135" s="0">
-        <v>0</v>
-      </c>
-      <c r="S135" s="0"/>
-      <c r="T135" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="S135" s="0" t="s">
+        <v>666</v>
+      </c>
+      <c r="T135" s="0" t="s">
+        <v>674</v>
+      </c>
       <c r="U135" s="0"/>
     </row>
     <row r="136">
@@ -25553,7 +25597,9 @@
       <c r="R385" s="0">
         <v>2</v>
       </c>
-      <c r="S385" s="0"/>
+      <c r="S385" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="T385" s="0" t="s">
         <v>39</v>
       </c>

</xml_diff>